<commit_message>
Pollen Zones to heatmap
</commit_message>
<xml_diff>
--- a/data/Pig_clustered_PC.xlsx
+++ b/data/Pig_clustered_PC.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t xml:space="preserve">Composite depth</t>
   </si>
@@ -81,6 +81,24 @@
   </si>
   <si>
     <t xml:space="preserve">PC4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">age</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AP2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AP1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HTM1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Younger Dryas</t>
   </si>
 </sst>
 </file>
@@ -482,6 +500,12 @@
       <c r="W1" t="s">
         <v>22</v>
       </c>
+      <c r="X1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -553,6 +577,12 @@
       <c r="W2" t="n">
         <v>1.09873683874954</v>
       </c>
+      <c r="X2" t="n">
+        <v>1577</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -624,6 +654,12 @@
       <c r="W3" t="n">
         <v>0.395379632063061</v>
       </c>
+      <c r="X3" t="n">
+        <v>1593</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -695,6 +731,10 @@
       <c r="W4" t="n">
         <v>0.330345480994295</v>
       </c>
+      <c r="X4" t="n">
+        <v>2375</v>
+      </c>
+      <c r="Y4"/>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -766,6 +806,12 @@
       <c r="W5" t="n">
         <v>0.0586357613351526</v>
       </c>
+      <c r="X5" t="n">
+        <v>3596</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -837,6 +883,12 @@
       <c r="W6" t="n">
         <v>0.0383531362365105</v>
       </c>
+      <c r="X6" t="n">
+        <v>3694</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -908,6 +960,12 @@
       <c r="W7" t="n">
         <v>0.0297186988073929</v>
       </c>
+      <c r="X7" t="n">
+        <v>3792</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -979,6 +1037,12 @@
       <c r="W8" t="n">
         <v>0.03603083457333</v>
       </c>
+      <c r="X8" t="n">
+        <v>4150</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -1050,6 +1114,12 @@
       <c r="W9" t="n">
         <v>0.061358272882746</v>
       </c>
+      <c r="X9" t="n">
+        <v>4361</v>
+      </c>
+      <c r="Y9" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -1121,6 +1191,10 @@
       <c r="W10" t="n">
         <v>0.0118202489816842</v>
       </c>
+      <c r="X10" t="n">
+        <v>4675</v>
+      </c>
+      <c r="Y10"/>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -1192,6 +1266,12 @@
       <c r="W11" t="n">
         <v>0.728847720846014</v>
       </c>
+      <c r="X11" t="n">
+        <v>9224</v>
+      </c>
+      <c r="Y11" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -1263,6 +1343,12 @@
       <c r="W12" t="n">
         <v>-2.16032620481767</v>
       </c>
+      <c r="X12" t="n">
+        <v>9337</v>
+      </c>
+      <c r="Y12" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -1334,6 +1420,12 @@
       <c r="W13" t="n">
         <v>-0.162569463056312</v>
       </c>
+      <c r="X13" t="n">
+        <v>9398</v>
+      </c>
+      <c r="Y13" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -1405,6 +1497,12 @@
       <c r="W14" t="n">
         <v>-0.924182484809314</v>
       </c>
+      <c r="X14" t="n">
+        <v>9467</v>
+      </c>
+      <c r="Y14" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -1476,6 +1574,10 @@
       <c r="W15" t="n">
         <v>-0.878053252623266</v>
       </c>
+      <c r="X15" t="n">
+        <v>10933</v>
+      </c>
+      <c r="Y15"/>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -1547,6 +1649,10 @@
       <c r="W16" t="n">
         <v>-0.351271188640038</v>
       </c>
+      <c r="X16" t="n">
+        <v>11012</v>
+      </c>
+      <c r="Y16"/>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -1618,6 +1724,10 @@
       <c r="W17" t="n">
         <v>-0.996455233977904</v>
       </c>
+      <c r="X17" t="n">
+        <v>11066</v>
+      </c>
+      <c r="Y17"/>
     </row>
     <row r="18">
       <c r="A18" t="n">
@@ -1689,6 +1799,10 @@
       <c r="W18" t="n">
         <v>0.627931846082416</v>
       </c>
+      <c r="X18" t="n">
+        <v>11184</v>
+      </c>
+      <c r="Y18"/>
     </row>
     <row r="19">
       <c r="A19" t="n">
@@ -1760,6 +1874,10 @@
       <c r="W19" t="n">
         <v>-0.0607490504833536</v>
       </c>
+      <c r="X19" t="n">
+        <v>11290</v>
+      </c>
+      <c r="Y19"/>
     </row>
     <row r="20">
       <c r="A20" t="n">
@@ -1831,6 +1949,12 @@
       <c r="W20" t="n">
         <v>0.781462780765576</v>
       </c>
+      <c r="X20" t="n">
+        <v>11901</v>
+      </c>
+      <c r="Y20" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
@@ -1902,6 +2026,12 @@
       <c r="W21" t="n">
         <v>-1.20836128571626</v>
       </c>
+      <c r="X21" t="n">
+        <v>12187</v>
+      </c>
+      <c r="Y21" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
@@ -1973,6 +2103,12 @@
       <c r="W22" t="n">
         <v>2.30730726269381</v>
       </c>
+      <c r="X22" t="n">
+        <v>12321</v>
+      </c>
+      <c r="Y22" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
@@ -2044,6 +2180,12 @@
       <c r="W23" t="n">
         <v>-1.21626913850119</v>
       </c>
+      <c r="X23" t="n">
+        <v>12441</v>
+      </c>
+      <c r="Y23" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
@@ -2114,6 +2256,12 @@
       </c>
       <c r="W24" t="n">
         <v>1.45230878761379</v>
+      </c>
+      <c r="X24" t="n">
+        <v>12630</v>
+      </c>
+      <c r="Y24" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>